<commit_message>
Updates after conversation with Keith
</commit_message>
<xml_diff>
--- a/Libraries/Health/Generated/MDMI Example Healthcare Domain Model Table.xlsx
+++ b/Libraries/Health/Generated/MDMI Example Healthcare Domain Model Table.xlsx
@@ -12,11 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="103">
   <si>
     <t/>
   </si>
   <si>
+    <t>Element ID</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -32,99 +35,180 @@
     <t>Documentation</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932667283_578110_6044</t>
+  </si>
+  <si>
     <t>allergic reaction observation</t>
   </si>
   <si>
     <t>allergic reaction</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932667284_121545_6045</t>
+  </si>
+  <si>
+    <t>_19_0_3_62501eb_1578694996433_774413_6726</t>
+  </si>
+  <si>
     <t>allergy opinion</t>
   </si>
   <si>
     <t>allergy</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1578694996434_437053_6727</t>
+  </si>
+  <si>
+    <t>_19_0_3_62501eb_1581105741408_455163_7331</t>
+  </si>
+  <si>
     <t>clinical activity</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1576171289956_933528_12331</t>
+  </si>
+  <si>
     <t>clinical situation</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932667401_681378_6304</t>
+  </si>
+  <si>
+    <t>_19_0_3_62501eb_1581439410653_635908_6762</t>
+  </si>
+  <si>
     <t>health related condition</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1581439888040_737322_6776</t>
+  </si>
+  <si>
     <t>medication</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575938781064_682315_11139</t>
+  </si>
+  <si>
     <t>medication activity</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1581442515746_351649_6834</t>
+  </si>
+  <si>
     <t>vital sign</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932667280_478117_6038</t>
+  </si>
+  <si>
     <t>vital sign observation</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932667280_396639_6039</t>
+  </si>
+  <si>
+    <t>_19_0_3_62501eb_1581439410653_264931_6761</t>
+  </si>
+  <si>
     <t>subject</t>
   </si>
   <si>
-    <t>condition of</t>
+    <t>_19_0_3_62501eb_1581442515746_256830_6833</t>
+  </si>
+  <si>
+    <t>_19_0_3_62501eb_1575938781063_864467_11138</t>
   </si>
   <si>
     <t>consumes</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1581115363833_428095_6704</t>
+  </si>
+  <si>
     <t>has dosage</t>
   </si>
   <si>
     <t>measure</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1581105619554_611153_7311</t>
+  </si>
+  <si>
     <t>has dose form</t>
   </si>
   <si>
     <t>reference</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1581105562224_754275_7303</t>
+  </si>
+  <si>
     <t>has ingredient</t>
   </si>
   <si>
     <t>substance</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1581105916125_511300_7348</t>
+  </si>
+  <si>
     <t>has location</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932667400_432786_6303</t>
+  </si>
+  <si>
     <t>has patient</t>
   </si>
   <si>
     <t>a property asserting what the clinicalstatement is about</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1581105641554_143458_7315</t>
+  </si>
+  <si>
     <t>has route</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1576171289955_293204_12330</t>
+  </si>
+  <si>
     <t>has site</t>
   </si>
   <si>
     <t>body location</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1581105588214_737974_7307</t>
+  </si>
+  <si>
     <t>has strength</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1576170905738_395553_12292</t>
+  </si>
+  <si>
     <t>has vital sigh value</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1581116150135_739112_6711</t>
+  </si>
+  <si>
     <t>laterality</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1581105741408_741963_7330</t>
+  </si>
+  <si>
     <t>uses device</t>
   </si>
   <si>
     <t>device</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932666937_126818_5370</t>
+  </si>
+  <si>
     <t>MDMI Example Healthcare Domain Model</t>
   </si>
   <si>
@@ -134,65 +218,111 @@
     <t>risk of harmful or undesirable, physiological response which is unique to an individual and associated with exposure to a substance.</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932666914_330525_5327</t>
+  </si>
+  <si>
     <t>observation</t>
   </si>
   <si>
     <t>a statementcontext property for a mdmibusinesselement</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1578694912303_354692_6680</t>
+  </si>
+  <si>
     <t>a bodies negative reaction to a substance</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1578694889873_510687_6655</t>
+  </si>
+  <si>
     <t>opinion</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932666853_60531_5213</t>
+  </si>
+  <si>
     <t>entity</t>
   </si>
   <si>
     <t>a class used in a dataelementconcept property</t>
+  </si>
+  <si>
+    <t>_19_0_3_62501eb_1576709459751_212403_6610</t>
   </si>
   <si>
     <t>activity
 clinical situation</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932666803_646860_5127</t>
+  </si>
+  <si>
     <t>situation</t>
   </si>
   <si>
     <t>a situation involving some process of healthcare.</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1576848426080_581998_6606</t>
+  </si>
+  <si>
     <t>consult</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932666920_674563_5339</t>
+  </si>
+  <si>
     <t>encounter</t>
   </si>
   <si>
     <t>an interaction between a patient and healthcare provider(s) for the purpose of providing healthcare service(s) or assessing the health status of a patient.</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1576101195264_864774_11895</t>
+  </si>
+  <si>
     <t>state of affairs</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932666733_316702_5026</t>
+  </si>
+  <si>
     <t>immunization activity</t>
   </si>
   <si>
     <t>describes the activty regarding a vaccine or a recording of an immunization as reported by a patient, a clinician or another party.</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575938749735_717594_11092</t>
+  </si>
+  <si>
     <t>a medication is a substance intended to improve a patient's condition</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1575932666846_481711_5201</t>
+  </si>
+  <si>
     <t>statements about medication activities; past, current, and future</t>
   </si>
   <si>
+    <t>_19_0_3_62501eb_1576709434181_966028_6577</t>
+  </si>
+  <si>
     <t>procedure</t>
   </si>
   <si>
-    <t>quality</t>
+    <t>_19_0_3_62501eb_1575932666765_847074_5072</t>
+  </si>
+  <si>
+    <t>quality
+health related condition</t>
   </si>
   <si>
     <t>a defined set up procedures resulting in observation</t>
+  </si>
+  <si>
+    <t>_19_0_3_62501eb_1575932666745_678311_5042</t>
   </si>
 </sst>
 </file>
@@ -262,27 +392,33 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -291,32 +427,38 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -325,15 +467,18 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -342,15 +487,18 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>0</v>
@@ -359,15 +507,18 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>0</v>
@@ -376,15 +527,18 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>0</v>
@@ -393,15 +547,18 @@
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>0</v>
@@ -410,15 +567,18 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>0</v>
@@ -427,15 +587,18 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>0</v>
@@ -444,32 +607,38 @@
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>0</v>
@@ -478,520 +647,613 @@
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>39</v>
+        <v>0</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>45</v>
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>54</v>
+        <v>0</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>55</v>
+        <v>0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>56</v>
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>59</v>
+        <v>0</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>